<commit_message>
Details page Heading changed as dinamic name
</commit_message>
<xml_diff>
--- a/OnlineAdmission.APP/wwwroot/FIleData/MBA.xlsx
+++ b/OnlineAdmission.APP/wwwroot/FIleData/MBA.xlsx
@@ -381,14 +381,14 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.140625" style="5" bestFit="1" customWidth="1"/>

</xml_diff>